<commit_message>
update presentation & gantt chart
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\data\home\mahmed1\Desktop_Windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omarfahmy/Desktop/HHN_Projects/CRV/CRV_Face_Detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2EC43B1-204D-4DE8-A740-33FDDD44A91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A3342A-1C43-B646-9323-55F86B2DA51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="500" windowWidth="21600" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="3" r:id="rId1"/>
@@ -26,9 +26,6 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -102,9 +99,6 @@
     <t>Polish results, finalize slides and demo, rehearse</t>
   </si>
   <si>
-    <t>Start writing report draft, start with the presentation slides</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tilting Detection Solution </t>
   </si>
   <si>
@@ -118,6 +112,9 @@
   </si>
   <si>
     <t>Comparision with a more up to date model (That needs no preprossesing)</t>
+  </si>
+  <si>
+    <t>Prepare the presentation slides</t>
   </si>
 </sst>
 </file>
@@ -474,9 +471,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -495,48 +489,51 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -552,9 +549,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -592,7 +589,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -698,7 +695,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -840,7 +837,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -854,111 +851,111 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
-    <col min="3" max="6" width="10.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="1" customWidth="1"/>
-    <col min="8" max="23" width="10.7109375" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="14.42578125" style="1"/>
+    <col min="1" max="1" width="2.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="1" customWidth="1"/>
+    <col min="3" max="6" width="10.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
+    <col min="8" max="23" width="10.6640625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="17" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="22"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="21"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31" t="s">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="25"/>
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="23" t="s">
+      <c r="G2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="33" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
     </row>
-    <row r="4" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -991,12 +988,12 @@
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
     </row>
-    <row r="5" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="11">
         <f>C4+7</f>
@@ -1025,12 +1022,12 @@
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
     </row>
-    <row r="6" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="11">
         <f>C5+7</f>
@@ -1043,11 +1040,11 @@
       <c r="E6" s="2">
         <v>3</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="35" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -1059,12 +1056,12 @@
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
     </row>
-    <row r="7" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="11">
         <f>D6-7</f>
@@ -1080,23 +1077,25 @@
       <c r="F7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="35"/>
+      <c r="K7" s="22"/>
       <c r="L7" s="15"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="11">
         <f>D7</f>
@@ -1112,22 +1111,24 @@
       <c r="F8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="16"/>
+      <c r="J8" s="10"/>
       <c r="K8" s="13"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="35"/>
+      <c r="N8" s="22"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="11">
         <f>C8</f>
@@ -1143,18 +1144,20 @@
       <c r="F9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="16"/>
+      <c r="L9" s="10"/>
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -1175,7 +1178,9 @@
       <c r="F10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="10"/>
@@ -1186,12 +1191,12 @@
       <c r="O10" s="10"/>
       <c r="P10" s="15"/>
     </row>
-    <row r="11" spans="1:16" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C11" s="11">
         <f>D9</f>
@@ -1199,34 +1204,29 @@
       </c>
       <c r="D11" s="11">
         <f t="shared" si="0"/>
-        <v>46027</v>
+        <v>46020</v>
       </c>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="16"/>
+      <c r="M11" s="10"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:G3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
@@ -1237,6 +1237,13 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="G4:G11">

</xml_diff>